<commit_message>
Moved some BoM components to Assembly BoM
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Qty</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>X17, X18, X19, X20, X21</t>
-  </si>
-  <si>
-    <t>Need contacts, wire, mating connectors, terminating connectors</t>
   </si>
 </sst>
 </file>
@@ -323,9 +320,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,6 +336,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -625,10 +622,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,17 +643,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -691,33 +688,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+    <row r="3" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>37</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="20"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>14</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
@@ -744,13 +741,13 @@
       <c r="A5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
@@ -775,13 +772,13 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
@@ -806,13 +803,13 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
@@ -837,22 +834,22 @@
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>40</v>
       </c>
       <c r="H8" s="10">
@@ -882,22 +879,22 @@
       <c r="A10" s="3">
         <v>15</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="10">
@@ -913,22 +910,22 @@
       <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="10">
@@ -944,7 +941,7 @@
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -975,7 +972,7 @@
       <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1006,7 +1003,7 @@
       <c r="A14" s="3">
         <v>1</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1037,7 +1034,7 @@
       <c r="A15" s="3">
         <v>5</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1065,31 +1062,22 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H16" s="10">
         <f>SUMPRODUCT(H3:H15,A3:A15)</f>
         <v>28.783000000000001</v>
       </c>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="10"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>